<commit_message>
update the message template
</commit_message>
<xml_diff>
--- a/Tools/address_raw_weight.xlsx
+++ b/Tools/address_raw_weight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xufei/Documents/GitHub/joeybot/Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230AAD23-60B6-3C4B-A56B-260BF48B9A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9875B02-4620-2948-B119-CCFDA920B552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32700" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>HwRnKq7RPtKHvX9wyHsc1zvfHtGjPQa5tyZtGtbvfXE</t>
   </si>
@@ -299,47 +299,47 @@
   </si>
   <si>
     <t>joe 新</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>vector的跟单号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>id</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>address</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>69ngexW9UkgRp5KFjLpaK9XNSCxUFmps6jYmqhK3q6m9</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>C5xCqdLR3ZGZ12AfawEfHUzAw8LMgHmWeP1JyAfGm5Xp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>G1pRtSyKuWSjTqRDcazzKBDzqEF96i1xSURpiXj3yFcc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Ay9wnuZCRTceZJuRpGZnuwYZuWdsviM4cMiCwFoSQiPH</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>CryptoD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>冷静</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Billy</t>
@@ -355,18 +355,63 @@
   </si>
   <si>
     <t>whale4</t>
+  </si>
+  <si>
+    <t>8tP391aDbKKpQS7eKnCEfnJ8Cmek6jatEe2LFkdJ2PRP</t>
+  </si>
+  <si>
+    <t>Jinmu</t>
+  </si>
+  <si>
+    <t>hu</t>
+  </si>
+  <si>
+    <t>joey</t>
+  </si>
+  <si>
+    <t>F7KSBM7SVVYUczJTCLpLJFPDEBrmrfi9ZiGru1BzAuwi</t>
+  </si>
+  <si>
+    <t>mai</t>
+  </si>
+  <si>
+    <t>杀破狼</t>
+  </si>
+  <si>
+    <t>ansem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -418,16 +463,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -719,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,7 +789,7 @@
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>94</v>
       </c>
@@ -741,8 +799,17 @@
       <c r="C1" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -752,8 +819,14 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -764,8 +837,14 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A55" si="0">A3+1</f>
         <v>3</v>
@@ -779,8 +858,14 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -794,8 +879,14 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -809,8 +900,14 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -821,8 +918,14 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -833,8 +936,14 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -845,8 +954,14 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -857,8 +972,17 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -869,8 +993,17 @@
       <c r="C11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -881,8 +1014,17 @@
       <c r="C12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -893,8 +1035,14 @@
       <c r="C13" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -905,8 +1053,14 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -917,8 +1071,14 @@
       <c r="C15" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -929,8 +1089,14 @@
       <c r="C16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -941,8 +1107,14 @@
       <c r="C17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -953,8 +1125,14 @@
       <c r="C18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -965,8 +1143,17 @@
       <c r="C19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -977,8 +1164,14 @@
       <c r="C20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -989,8 +1182,14 @@
       <c r="C21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1001,8 +1200,14 @@
       <c r="C22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1013,8 +1218,14 @@
       <c r="C23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1025,8 +1236,14 @@
       <c r="C24" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1040,8 +1257,14 @@
       <c r="D25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1052,8 +1275,14 @@
       <c r="C26" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1067,8 +1296,14 @@
       <c r="D27">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1079,8 +1314,14 @@
       <c r="C28" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1094,8 +1335,14 @@
       <c r="D29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1106,8 +1353,14 @@
       <c r="C30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1118,8 +1371,14 @@
       <c r="C31" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1130,8 +1389,14 @@
       <c r="C32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1142,8 +1407,14 @@
       <c r="C33" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1154,8 +1425,14 @@
       <c r="C34" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1166,8 +1443,17 @@
       <c r="C35" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1178,8 +1464,14 @@
       <c r="C36" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1190,8 +1482,17 @@
       <c r="C37" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1202,8 +1503,17 @@
       <c r="C38" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1214,8 +1524,17 @@
       <c r="C39" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1229,8 +1548,14 @@
       <c r="D40">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1241,8 +1566,17 @@
       <c r="C41" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1253,8 +1587,17 @@
       <c r="C42" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1265,8 +1608,17 @@
       <c r="C43" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="F43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1277,8 +1629,14 @@
       <c r="C44" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1292,8 +1650,14 @@
       <c r="D45">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1304,8 +1668,17 @@
       <c r="C46" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1316,8 +1689,17 @@
       <c r="C47" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1331,8 +1713,14 @@
       <c r="D48">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>9</v>
+      </c>
+      <c r="F48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1346,8 +1734,14 @@
       <c r="D49">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1361,8 +1755,14 @@
       <c r="D50">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1376,8 +1776,14 @@
       <c r="D51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52">
         <f>A51+1</f>
         <v>51</v>
@@ -1388,8 +1794,17 @@
       <c r="C52" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>9</v>
+      </c>
+      <c r="E52">
+        <v>10</v>
+      </c>
+      <c r="F52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1403,8 +1818,14 @@
       <c r="D53">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>10</v>
+      </c>
+      <c r="F53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1418,8 +1839,14 @@
       <c r="D54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1433,15 +1860,59 @@
       <c r="D55">
         <v>5</v>
       </c>
+      <c r="E55">
+        <v>5</v>
+      </c>
+      <c r="F55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56">
+        <v>7</v>
+      </c>
+      <c r="E56">
+        <v>7</v>
+      </c>
+      <c r="F56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C58" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:B55">
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to chainsmonitor version
</commit_message>
<xml_diff>
--- a/Tools/address_raw_weight.xlsx
+++ b/Tools/address_raw_weight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xufei/Documents/GitHub/joeybot/Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9875B02-4620-2948-B119-CCFDA920B552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4DC7B5-EC5A-2045-840B-A7B219B15ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32700" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
   <si>
     <t>HwRnKq7RPtKHvX9wyHsc1zvfHtGjPQa5tyZtGtbvfXE</t>
   </si>
@@ -299,47 +299,47 @@
   </si>
   <si>
     <t>joe 新</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>vector的跟单号</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>id</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>address</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>69ngexW9UkgRp5KFjLpaK9XNSCxUFmps6jYmqhK3q6m9</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>C5xCqdLR3ZGZ12AfawEfHUzAw8LMgHmWeP1JyAfGm5Xp</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>G1pRtSyKuWSjTqRDcazzKBDzqEF96i1xSURpiXj3yFcc</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Ay9wnuZCRTceZJuRpGZnuwYZuWdsviM4cMiCwFoSQiPH</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CryptoD</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>冷静</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Billy</t>
@@ -379,18 +379,49 @@
   </si>
   <si>
     <t>ansem</t>
+  </si>
+  <si>
+    <t>AVAZvHLR2PcWpDf8BXY4rVxNHYRBytycHkcB5z5QNXYm</t>
+  </si>
+  <si>
+    <t>川沐</t>
+  </si>
+  <si>
+    <t>CdFjn99C4VUjpqayV4fnf2w5JUiF254LJTamkhdwEqqT</t>
+  </si>
+  <si>
+    <t>4rUVt2HPSPQEUdDbk21d4hXP9AGiG8kBKnJ1c4mLKaD3</t>
+  </si>
+  <si>
+    <t>奶子哥</t>
+  </si>
+  <si>
+    <t>EUM51CoFuxBw2FUVQ7YmrAy6a3p6PUNwou5S9f8qt83S</t>
+  </si>
+  <si>
+    <t>大宇</t>
+  </si>
+  <si>
+    <t>score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -463,14 +494,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,19 +810,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="61.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="3" max="4" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>94</v>
       </c>
@@ -799,17 +832,20 @@
       <c r="C1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -819,14 +855,21 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="8">
+        <f>AVERAGE(E2:G2)</f>
+        <v>4</v>
+      </c>
       <c r="E2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -837,16 +880,23 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D61" si="0">AVERAGE(E3:G3)</f>
+        <v>6.333333333333333</v>
+      </c>
       <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
         <v>7</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f t="shared" ref="A4:A55" si="0">A3+1</f>
+        <f t="shared" ref="A4:A55" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -855,19 +905,23 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -876,19 +930,23 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -897,19 +955,23 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
-        <v>1</v>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -918,16 +980,23 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>4.666666666666667</v>
+      </c>
       <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
         <v>7</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -936,16 +1005,23 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
+      <c r="D8" s="8">
+        <f t="shared" si="0"/>
+        <v>4.666666666666667</v>
+      </c>
       <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -954,16 +1030,23 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
+      <c r="D9" s="8">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666665</v>
+      </c>
       <c r="E9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -972,19 +1055,23 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
-        <v>5</v>
+      <c r="D10" s="8">
+        <f t="shared" si="0"/>
+        <v>5.666666666666667</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -993,7 +1080,8 @@
       <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E11">
@@ -1002,10 +1090,13 @@
       <c r="F11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1014,7 +1105,8 @@
       <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E12">
@@ -1023,10 +1115,13 @@
       <c r="F12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1035,16 +1130,23 @@
       <c r="C13" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1053,16 +1155,23 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>3</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1071,16 +1180,23 @@
       <c r="C15" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="D15" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>3</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1089,16 +1205,23 @@
       <c r="C16" t="s">
         <v>25</v>
       </c>
+      <c r="D16" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
       <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
         <v>2</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1107,16 +1230,23 @@
       <c r="C17" t="s">
         <v>27</v>
       </c>
+      <c r="D17" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
         <v>3</v>
       </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1125,16 +1255,23 @@
       <c r="C18" t="s">
         <v>29</v>
       </c>
+      <c r="D18" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="E18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1143,7 +1280,8 @@
       <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="8">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E19">
@@ -1152,10 +1290,13 @@
       <c r="F19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1164,16 +1305,23 @@
       <c r="C20" t="s">
         <v>33</v>
       </c>
+      <c r="D20" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="E20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1182,16 +1330,23 @@
       <c r="C21" t="s">
         <v>35</v>
       </c>
+      <c r="D21" s="8">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1200,16 +1355,23 @@
       <c r="C22" t="s">
         <v>37</v>
       </c>
+      <c r="D22" s="8">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1218,16 +1380,23 @@
       <c r="C23" t="s">
         <v>39</v>
       </c>
+      <c r="D23" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1236,16 +1405,23 @@
       <c r="C24" t="s">
         <v>41</v>
       </c>
+      <c r="D24" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1254,19 +1430,23 @@
       <c r="C25" t="s">
         <v>43</v>
       </c>
-      <c r="D25">
-        <v>1</v>
+      <c r="D25" s="8">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1275,16 +1455,23 @@
       <c r="C26" t="s">
         <v>45</v>
       </c>
+      <c r="D26" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
         <v>4</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1293,7 +1480,8 @@
       <c r="C27" t="s">
         <v>47</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="8">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E27">
@@ -1302,10 +1490,13 @@
       <c r="F27">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1314,16 +1505,23 @@
       <c r="C28" t="s">
         <v>51</v>
       </c>
+      <c r="D28" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
         <v>4</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1332,19 +1530,23 @@
       <c r="C29" t="s">
         <v>53</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="8">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="E29">
         <v>9</v>
-      </c>
-      <c r="E29">
-        <v>10</v>
       </c>
       <c r="F29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1353,16 +1555,23 @@
       <c r="C30" t="s">
         <v>49</v>
       </c>
+      <c r="D30" s="8">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1371,16 +1580,23 @@
       <c r="C31" t="s">
         <v>55</v>
       </c>
+      <c r="D31" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
         <v>2</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1389,16 +1605,23 @@
       <c r="C32" t="s">
         <v>57</v>
       </c>
+      <c r="D32" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="E32">
         <v>3</v>
       </c>
       <c r="F32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1407,16 +1630,23 @@
       <c r="C33" t="s">
         <v>59</v>
       </c>
+      <c r="D33" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
         <v>4</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1425,16 +1655,23 @@
       <c r="C34" t="s">
         <v>61</v>
       </c>
+      <c r="D34" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
         <v>3</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1443,19 +1680,23 @@
       <c r="C35" t="s">
         <v>63</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="8">
+        <f t="shared" si="0"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="E35">
         <v>6</v>
       </c>
-      <c r="E35">
-        <v>5</v>
-      </c>
       <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1464,16 +1705,23 @@
       <c r="C36" t="s">
         <v>65</v>
       </c>
+      <c r="D36" s="8">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
       <c r="E36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1482,7 +1730,8 @@
       <c r="C37" t="s">
         <v>67</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="8">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E37">
@@ -1491,10 +1740,13 @@
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1503,19 +1755,23 @@
       <c r="C38" t="s">
         <v>69</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="8">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="E38">
         <v>2</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>3</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1524,19 +1780,23 @@
       <c r="C39" t="s">
         <v>71</v>
       </c>
-      <c r="D39">
-        <v>2</v>
+      <c r="D39" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
       <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1545,19 +1805,23 @@
       <c r="C40" t="s">
         <v>73</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="8">
+        <f t="shared" si="0"/>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="E40">
         <v>8</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>7</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1566,19 +1830,23 @@
       <c r="C41" t="s">
         <v>75</v>
       </c>
-      <c r="D41">
-        <v>1</v>
+      <c r="D41" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
         <v>3</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1587,19 +1855,23 @@
       <c r="C42" t="s">
         <v>77</v>
       </c>
-      <c r="D42">
-        <v>2</v>
+      <c r="D42" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="E42">
         <v>2</v>
       </c>
       <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1608,19 +1880,23 @@
       <c r="C43" t="s">
         <v>79</v>
       </c>
-      <c r="D43">
-        <v>8</v>
+      <c r="D43" s="8">
+        <f t="shared" si="0"/>
+        <v>7.666666666666667</v>
       </c>
       <c r="E43">
         <v>8</v>
       </c>
       <c r="F43">
+        <v>8</v>
+      </c>
+      <c r="G43">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1629,16 +1905,23 @@
       <c r="C44" t="s">
         <v>81</v>
       </c>
+      <c r="D44" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
         <v>4</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1647,7 +1930,8 @@
       <c r="C45" t="s">
         <v>83</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="8">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E45">
@@ -1656,10 +1940,13 @@
       <c r="F45">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1668,19 +1955,23 @@
       <c r="C46" t="s">
         <v>85</v>
       </c>
-      <c r="D46">
-        <v>3</v>
+      <c r="D46" s="8">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
       <c r="F46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1689,19 +1980,23 @@
       <c r="C47" t="s">
         <v>87</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="8">
+        <f t="shared" si="0"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="E47">
         <v>6</v>
       </c>
-      <c r="E47">
-        <v>5</v>
-      </c>
       <c r="F47">
+        <v>5</v>
+      </c>
+      <c r="G47">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1710,19 +2005,23 @@
       <c r="C48" t="s">
         <v>89</v>
       </c>
-      <c r="D48">
-        <v>9</v>
+      <c r="D48" s="8">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333339</v>
       </c>
       <c r="E48">
         <v>9</v>
       </c>
       <c r="F48">
+        <v>9</v>
+      </c>
+      <c r="G48">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1731,19 +2030,23 @@
       <c r="C49" t="s">
         <v>91</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E49">
         <v>9</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>4</v>
       </c>
-      <c r="F49">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1752,19 +2055,23 @@
       <c r="C50" s="2">
         <v>69</v>
       </c>
-      <c r="D50">
-        <v>8</v>
+      <c r="D50" s="8">
+        <f t="shared" si="0"/>
+        <v>7.666666666666667</v>
       </c>
       <c r="E50">
         <v>8</v>
       </c>
       <c r="F50">
+        <v>8</v>
+      </c>
+      <c r="G50">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1773,17 +2080,21 @@
       <c r="C51" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D51">
-        <v>5</v>
+      <c r="D51" s="8">
+        <f t="shared" si="0"/>
+        <v>5.666666666666667</v>
       </c>
       <c r="E51">
         <v>5</v>
       </c>
       <c r="F51">
+        <v>5</v>
+      </c>
+      <c r="G51">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A52">
         <f>A51+1</f>
         <v>51</v>
@@ -1794,19 +2105,23 @@
       <c r="C52" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="8">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="E52">
         <v>9</v>
-      </c>
-      <c r="E52">
-        <v>10</v>
       </c>
       <c r="F52">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1815,7 +2130,8 @@
       <c r="C53" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="8">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E53">
@@ -1824,10 +2140,13 @@
       <c r="F53">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" t="s">
@@ -1836,7 +2155,8 @@
       <c r="C54" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="8">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E54">
@@ -1845,10 +2165,13 @@
       <c r="F54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" t="s">
@@ -1857,17 +2180,21 @@
       <c r="C55" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D55">
-        <v>5</v>
+      <c r="D55" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E55">
         <v>5</v>
       </c>
       <c r="F55">
+        <v>5</v>
+      </c>
+      <c r="G55">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1877,37 +2204,148 @@
       <c r="C56" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D56">
-        <v>7</v>
+      <c r="D56" s="8">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
       </c>
       <c r="E56">
         <v>7</v>
       </c>
       <c r="F56">
+        <v>7</v>
+      </c>
+      <c r="G56">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
       <c r="B57" t="s">
         <v>112</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D57">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D57" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>5</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="C58" s="6" t="s">
         <v>115</v>
       </c>
+      <c r="D58" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E58">
+        <v>7</v>
+      </c>
+      <c r="F58">
+        <v>6</v>
+      </c>
+      <c r="G58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="8">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="E59">
+        <v>9</v>
+      </c>
+      <c r="F59">
+        <v>7.5</v>
+      </c>
+      <c r="G59">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D60" s="8">
+        <f t="shared" si="0"/>
+        <v>7.833333333333333</v>
+      </c>
+      <c r="E60">
+        <v>8</v>
+      </c>
+      <c r="F60">
+        <v>7.5</v>
+      </c>
+      <c r="G60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D61" s="8">
+        <f t="shared" si="0"/>
+        <v>7.833333333333333</v>
+      </c>
+      <c r="E61">
+        <v>8</v>
+      </c>
+      <c r="F61">
+        <v>7.5</v>
+      </c>
+      <c r="G61">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D64" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:B55">
     <cfRule type="duplicateValues" dxfId="0" priority="8"/>

</xml_diff>